<commit_message>
add_new_item function corrected and now working as intended. Next step should be to add checking for duplicate already in inventory followed by a function for removing items and reorganizing the inventory
</commit_message>
<xml_diff>
--- a/CRAPveg.xlsx
+++ b/CRAPveg.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,7 +451,7 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Type.1</t>
+          <t>Type.</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -758,7 +758,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Butter?</t>
+          <t>Yellow Butterwax</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -983,7 +983,7 @@
       </c>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="n">
-        <v>74</v>
+        <v>20</v>
       </c>
       <c r="F21" t="n">
         <v>2.99</v>
@@ -1059,6 +1059,78 @@
       </c>
       <c r="F24" t="n">
         <v>2.99</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Veg</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Bean</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Orca</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="n">
+        <v>24</v>
+      </c>
+      <c r="F25" t="n">
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Veg</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Watermelon</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Sugar Baby</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" t="n">
+        <v>15</v>
+      </c>
+      <c r="F26" t="n">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Veg</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Peas</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Sweet Magnolia</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr"/>
+      <c r="E27" t="n">
+        <v>25</v>
+      </c>
+      <c r="F27" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added change price in inventory, put in change_name and change_variety as place holders for code.
</commit_message>
<xml_diff>
--- a/CRAPveg.xlsx
+++ b/CRAPveg.xlsx
@@ -1103,10 +1103,10 @@
       </c>
       <c r="D26" t="inlineStr"/>
       <c r="E26" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F26" t="n">
-        <v>8.5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27">

</xml_diff>